<commit_message>
backup as on 15th may
</commit_message>
<xml_diff>
--- a/uploads/Copy of questions2.xlsx
+++ b/uploads/Copy of questions2.xlsx
@@ -9,7 +9,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SUNIDHI HARRISON\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716779EA-83BF-42DC-940E-C8CCFA361ACE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66B2221-635D-4CEB-9E61-D6C529EA2D18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="82">
   <si>
     <t>What is the average of first five multiples of 12?</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Basic</t>
   </si>
   <si>
-    <t>Intermediate</t>
-  </si>
-  <si>
     <t>What is the difference in the place value of 5 in the numeral 754853?</t>
   </si>
   <si>
@@ -211,21 +208,12 @@
     <t>Category</t>
   </si>
   <si>
-    <t>BTCSE501</t>
-  </si>
-  <si>
     <t>Artificial Intelligence</t>
   </si>
   <si>
-    <t>B.Tech</t>
-  </si>
-  <si>
     <t>xyz</t>
   </si>
   <si>
-    <t>mno</t>
-  </si>
-  <si>
     <t>Rs. 230</t>
   </si>
   <si>
@@ -245,6 +233,42 @@
   </si>
   <si>
     <t>18 hours</t>
+  </si>
+  <si>
+    <t>BCA101</t>
+  </si>
+  <si>
+    <t>BCA102</t>
+  </si>
+  <si>
+    <t>BCA103</t>
+  </si>
+  <si>
+    <t>C Programming</t>
+  </si>
+  <si>
+    <t>BCA</t>
+  </si>
+  <si>
+    <t>Circuit Theory</t>
+  </si>
+  <si>
+    <t>Computer Networks</t>
+  </si>
+  <si>
+    <t>BCA201</t>
+  </si>
+  <si>
+    <t>BCA202</t>
+  </si>
+  <si>
+    <t>BCA203</t>
+  </si>
+  <si>
+    <t>Data Mining</t>
+  </si>
+  <si>
+    <t>Java</t>
   </si>
 </sst>
 </file>
@@ -640,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U12"/>
+  <dimension ref="A1:U67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T35" sqref="T35:T45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -661,67 +685,67 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" t="s">
         <v>55</v>
       </c>
-      <c r="D1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" t="s">
         <v>46</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>53</v>
       </c>
-      <c r="L1" t="s">
-        <v>56</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" t="s">
+        <v>60</v>
+      </c>
+      <c r="S1" t="s">
+        <v>59</v>
+      </c>
+      <c r="T1" t="s">
         <v>57</v>
       </c>
-      <c r="N1" t="s">
-        <v>47</v>
-      </c>
-      <c r="O1" t="s">
-        <v>54</v>
-      </c>
-      <c r="P1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>49</v>
-      </c>
-      <c r="R1" t="s">
-        <v>61</v>
-      </c>
-      <c r="S1" t="s">
-        <v>60</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>58</v>
-      </c>
-      <c r="U1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
@@ -757,16 +781,16 @@
         <v>1</v>
       </c>
       <c r="R2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S2" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="T2" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="U2" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
@@ -774,7 +798,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="2">
@@ -807,16 +831,16 @@
         <v>1</v>
       </c>
       <c r="R3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S3" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="T3" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="U3" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
@@ -824,31 +848,31 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P4">
         <v>1</v>
@@ -857,16 +881,16 @@
         <v>1</v>
       </c>
       <c r="R4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S4" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="T4" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="U4" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
@@ -874,31 +898,31 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P5">
         <v>1</v>
@@ -907,16 +931,16 @@
         <v>1</v>
       </c>
       <c r="R5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S5" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="T5" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="U5" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
@@ -924,31 +948,31 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P6">
         <v>1</v>
@@ -957,16 +981,16 @@
         <v>1</v>
       </c>
       <c r="R6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="S6" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="T6" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="U6" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -974,31 +998,31 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P7">
         <v>1</v>
@@ -1007,16 +1031,16 @@
         <v>1</v>
       </c>
       <c r="R7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="S7" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="T7" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="U7" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
@@ -1024,31 +1048,31 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P8">
         <v>1</v>
@@ -1057,16 +1081,16 @@
         <v>1</v>
       </c>
       <c r="R8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="S8" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="T8" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="U8" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
@@ -1074,7 +1098,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9">
@@ -1102,16 +1126,16 @@
         <v>1</v>
       </c>
       <c r="R9" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="S9" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="T9" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="U9" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
@@ -1119,31 +1143,31 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P10">
         <v>1</v>
@@ -1152,16 +1176,16 @@
         <v>1</v>
       </c>
       <c r="R10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="S10" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="T10" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="U10" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
@@ -1169,7 +1193,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11">
@@ -1197,16 +1221,16 @@
         <v>1</v>
       </c>
       <c r="R11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="S11" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="T11" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="U11" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
@@ -1214,49 +1238,2520 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>1</v>
+      </c>
+      <c r="R12" t="s">
+        <v>62</v>
+      </c>
+      <c r="S12" t="s">
+        <v>70</v>
+      </c>
+      <c r="T12" t="s">
+        <v>73</v>
+      </c>
+      <c r="U12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>36</v>
+      </c>
+      <c r="F13">
         <v>38</v>
       </c>
-      <c r="P12">
-        <v>1</v>
-      </c>
-      <c r="Q12" t="s">
+      <c r="H13">
+        <v>40</v>
+      </c>
+      <c r="J13">
+        <v>42</v>
+      </c>
+      <c r="L13">
+        <v>44</v>
+      </c>
+      <c r="N13">
+        <v>36</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>1</v>
+      </c>
+      <c r="R13" t="s">
+        <v>62</v>
+      </c>
+      <c r="S13" t="s">
+        <v>71</v>
+      </c>
+      <c r="T13" t="s">
+        <v>75</v>
+      </c>
+      <c r="U13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="R12" t="s">
+      <c r="D14" s="2">
+        <v>49500</v>
+      </c>
+      <c r="F14" s="2">
+        <v>49950</v>
+      </c>
+      <c r="H14" s="2">
+        <v>45000</v>
+      </c>
+      <c r="J14" s="2">
+        <v>49940</v>
+      </c>
+      <c r="L14" s="2">
+        <v>45990</v>
+      </c>
+      <c r="N14" s="2">
+        <v>49950</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>1</v>
+      </c>
+      <c r="R14" t="s">
+        <v>62</v>
+      </c>
+      <c r="S14" t="s">
+        <v>71</v>
+      </c>
+      <c r="T14" t="s">
+        <v>75</v>
+      </c>
+      <c r="U14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>1</v>
+      </c>
+      <c r="R15" t="s">
+        <v>62</v>
+      </c>
+      <c r="S15" t="s">
+        <v>71</v>
+      </c>
+      <c r="T15" t="s">
+        <v>75</v>
+      </c>
+      <c r="U15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>1</v>
+      </c>
+      <c r="R16" t="s">
+        <v>62</v>
+      </c>
+      <c r="S16" t="s">
+        <v>71</v>
+      </c>
+      <c r="T16" t="s">
+        <v>75</v>
+      </c>
+      <c r="U16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>1</v>
+      </c>
+      <c r="R17" t="s">
+        <v>62</v>
+      </c>
+      <c r="S17" t="s">
+        <v>71</v>
+      </c>
+      <c r="T17" t="s">
+        <v>75</v>
+      </c>
+      <c r="U17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="S12" t="s">
-        <v>62</v>
-      </c>
-      <c r="T12" t="s">
+      <c r="N18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>1</v>
+      </c>
+      <c r="R18" t="s">
+        <v>62</v>
+      </c>
+      <c r="S18" t="s">
+        <v>71</v>
+      </c>
+      <c r="T18" t="s">
+        <v>75</v>
+      </c>
+      <c r="U18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>1</v>
+      </c>
+      <c r="R19" t="s">
+        <v>62</v>
+      </c>
+      <c r="S19" t="s">
+        <v>71</v>
+      </c>
+      <c r="T19" t="s">
+        <v>75</v>
+      </c>
+      <c r="U19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20">
+        <v>24</v>
+      </c>
+      <c r="F20">
+        <v>22</v>
+      </c>
+      <c r="H20">
+        <v>23</v>
+      </c>
+      <c r="J20">
+        <v>21</v>
+      </c>
+      <c r="L20">
+        <v>20</v>
+      </c>
+      <c r="N20">
+        <v>22</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>1</v>
+      </c>
+      <c r="R20" t="s">
+        <v>62</v>
+      </c>
+      <c r="S20" t="s">
+        <v>71</v>
+      </c>
+      <c r="T20" t="s">
+        <v>75</v>
+      </c>
+      <c r="U20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>1</v>
+      </c>
+      <c r="R21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S21" t="s">
+        <v>71</v>
+      </c>
+      <c r="T21" t="s">
+        <v>75</v>
+      </c>
+      <c r="U21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22">
+        <v>112</v>
+      </c>
+      <c r="F22">
+        <v>116</v>
+      </c>
+      <c r="H22">
+        <v>115</v>
+      </c>
+      <c r="J22">
+        <v>120</v>
+      </c>
+      <c r="L22">
+        <v>118</v>
+      </c>
+      <c r="N22">
+        <v>112</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>1</v>
+      </c>
+      <c r="R22" t="s">
+        <v>62</v>
+      </c>
+      <c r="S22" t="s">
+        <v>71</v>
+      </c>
+      <c r="T22" t="s">
+        <v>75</v>
+      </c>
+      <c r="U22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>1</v>
+      </c>
+      <c r="R23" t="s">
+        <v>62</v>
+      </c>
+      <c r="S23" t="s">
+        <v>71</v>
+      </c>
+      <c r="T23" t="s">
+        <v>75</v>
+      </c>
+      <c r="U23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>36</v>
+      </c>
+      <c r="F24">
+        <v>38</v>
+      </c>
+      <c r="H24">
+        <v>40</v>
+      </c>
+      <c r="J24">
+        <v>42</v>
+      </c>
+      <c r="L24">
+        <v>44</v>
+      </c>
+      <c r="N24">
+        <v>36</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>1</v>
+      </c>
+      <c r="R24" t="s">
+        <v>62</v>
+      </c>
+      <c r="S24" t="s">
+        <v>72</v>
+      </c>
+      <c r="T24" t="s">
+        <v>76</v>
+      </c>
+      <c r="U24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="2">
+        <v>49500</v>
+      </c>
+      <c r="F25" s="2">
+        <v>49950</v>
+      </c>
+      <c r="H25" s="2">
+        <v>45000</v>
+      </c>
+      <c r="J25" s="2">
+        <v>49940</v>
+      </c>
+      <c r="L25" s="2">
+        <v>45990</v>
+      </c>
+      <c r="N25" s="2">
+        <v>49950</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>1</v>
+      </c>
+      <c r="R25" t="s">
+        <v>62</v>
+      </c>
+      <c r="S25" t="s">
+        <v>72</v>
+      </c>
+      <c r="T25" t="s">
+        <v>76</v>
+      </c>
+      <c r="U25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L26" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="U12" t="s">
+      <c r="N26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>1</v>
+      </c>
+      <c r="R26" t="s">
+        <v>62</v>
+      </c>
+      <c r="S26" t="s">
+        <v>72</v>
+      </c>
+      <c r="T26" t="s">
+        <v>76</v>
+      </c>
+      <c r="U26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L27" s="2" t="s">
         <v>64</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>1</v>
+      </c>
+      <c r="R27" t="s">
+        <v>62</v>
+      </c>
+      <c r="S27" t="s">
+        <v>72</v>
+      </c>
+      <c r="T27" t="s">
+        <v>76</v>
+      </c>
+      <c r="U27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P28">
+        <v>1</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>1</v>
+      </c>
+      <c r="R28" t="s">
+        <v>62</v>
+      </c>
+      <c r="S28" t="s">
+        <v>72</v>
+      </c>
+      <c r="T28" t="s">
+        <v>76</v>
+      </c>
+      <c r="U28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P29">
+        <v>1</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>1</v>
+      </c>
+      <c r="R29" t="s">
+        <v>62</v>
+      </c>
+      <c r="S29" t="s">
+        <v>72</v>
+      </c>
+      <c r="T29" t="s">
+        <v>76</v>
+      </c>
+      <c r="U29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P30">
+        <v>1</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>1</v>
+      </c>
+      <c r="R30" t="s">
+        <v>62</v>
+      </c>
+      <c r="S30" t="s">
+        <v>72</v>
+      </c>
+      <c r="T30" t="s">
+        <v>76</v>
+      </c>
+      <c r="U30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31">
+        <v>24</v>
+      </c>
+      <c r="F31">
+        <v>22</v>
+      </c>
+      <c r="H31">
+        <v>23</v>
+      </c>
+      <c r="J31">
+        <v>21</v>
+      </c>
+      <c r="L31">
+        <v>20</v>
+      </c>
+      <c r="N31">
+        <v>22</v>
+      </c>
+      <c r="P31">
+        <v>1</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>1</v>
+      </c>
+      <c r="R31" t="s">
+        <v>62</v>
+      </c>
+      <c r="S31" t="s">
+        <v>72</v>
+      </c>
+      <c r="T31" t="s">
+        <v>76</v>
+      </c>
+      <c r="U31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P32">
+        <v>1</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>1</v>
+      </c>
+      <c r="R32" t="s">
+        <v>62</v>
+      </c>
+      <c r="S32" t="s">
+        <v>72</v>
+      </c>
+      <c r="T32" t="s">
+        <v>76</v>
+      </c>
+      <c r="U32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33">
+        <v>112</v>
+      </c>
+      <c r="F33">
+        <v>116</v>
+      </c>
+      <c r="H33">
+        <v>115</v>
+      </c>
+      <c r="J33">
+        <v>120</v>
+      </c>
+      <c r="L33">
+        <v>118</v>
+      </c>
+      <c r="N33">
+        <v>112</v>
+      </c>
+      <c r="P33">
+        <v>1</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>1</v>
+      </c>
+      <c r="R33" t="s">
+        <v>62</v>
+      </c>
+      <c r="S33" t="s">
+        <v>72</v>
+      </c>
+      <c r="T33" t="s">
+        <v>76</v>
+      </c>
+      <c r="U33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P34">
+        <v>1</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>1</v>
+      </c>
+      <c r="R34" t="s">
+        <v>62</v>
+      </c>
+      <c r="S34" t="s">
+        <v>72</v>
+      </c>
+      <c r="T34" t="s">
+        <v>76</v>
+      </c>
+      <c r="U34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35">
+        <v>36</v>
+      </c>
+      <c r="F35">
+        <v>38</v>
+      </c>
+      <c r="H35">
+        <v>40</v>
+      </c>
+      <c r="J35">
+        <v>42</v>
+      </c>
+      <c r="L35">
+        <v>44</v>
+      </c>
+      <c r="N35">
+        <v>36</v>
+      </c>
+      <c r="P35">
+        <v>1</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>1</v>
+      </c>
+      <c r="R35" t="s">
+        <v>62</v>
+      </c>
+      <c r="S35" t="s">
+        <v>77</v>
+      </c>
+      <c r="T35" t="s">
+        <v>81</v>
+      </c>
+      <c r="U35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="2">
+        <v>49500</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2">
+        <v>49950</v>
+      </c>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2">
+        <v>45000</v>
+      </c>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2">
+        <v>49940</v>
+      </c>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2">
+        <v>45990</v>
+      </c>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2">
+        <v>49950</v>
+      </c>
+      <c r="P36">
+        <v>1</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>1</v>
+      </c>
+      <c r="R36" t="s">
+        <v>62</v>
+      </c>
+      <c r="S36" t="s">
+        <v>77</v>
+      </c>
+      <c r="T36" t="s">
+        <v>81</v>
+      </c>
+      <c r="U36" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P37">
+        <v>1</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>1</v>
+      </c>
+      <c r="R37" t="s">
+        <v>62</v>
+      </c>
+      <c r="S37" t="s">
+        <v>77</v>
+      </c>
+      <c r="T37" t="s">
+        <v>81</v>
+      </c>
+      <c r="U37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P38">
+        <v>1</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>1</v>
+      </c>
+      <c r="R38" t="s">
+        <v>62</v>
+      </c>
+      <c r="S38" t="s">
+        <v>77</v>
+      </c>
+      <c r="T38" t="s">
+        <v>81</v>
+      </c>
+      <c r="U38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P39">
+        <v>1</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>1</v>
+      </c>
+      <c r="R39" t="s">
+        <v>62</v>
+      </c>
+      <c r="S39" t="s">
+        <v>77</v>
+      </c>
+      <c r="T39" t="s">
+        <v>81</v>
+      </c>
+      <c r="U39" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P40">
+        <v>1</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>1</v>
+      </c>
+      <c r="R40" t="s">
+        <v>62</v>
+      </c>
+      <c r="S40" t="s">
+        <v>77</v>
+      </c>
+      <c r="T40" t="s">
+        <v>81</v>
+      </c>
+      <c r="U40" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P41">
+        <v>1</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>1</v>
+      </c>
+      <c r="R41" t="s">
+        <v>62</v>
+      </c>
+      <c r="S41" t="s">
+        <v>77</v>
+      </c>
+      <c r="T41" t="s">
+        <v>81</v>
+      </c>
+      <c r="U41" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="D42">
+        <v>24</v>
+      </c>
+      <c r="F42">
+        <v>22</v>
+      </c>
+      <c r="H42">
+        <v>23</v>
+      </c>
+      <c r="J42">
+        <v>21</v>
+      </c>
+      <c r="L42">
+        <v>20</v>
+      </c>
+      <c r="N42">
+        <v>22</v>
+      </c>
+      <c r="P42">
+        <v>1</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>1</v>
+      </c>
+      <c r="R42" t="s">
+        <v>62</v>
+      </c>
+      <c r="S42" t="s">
+        <v>77</v>
+      </c>
+      <c r="T42" t="s">
+        <v>81</v>
+      </c>
+      <c r="U42" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43" s="1"/>
+      <c r="D43" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P43">
+        <v>1</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>1</v>
+      </c>
+      <c r="R43" t="s">
+        <v>62</v>
+      </c>
+      <c r="S43" t="s">
+        <v>77</v>
+      </c>
+      <c r="T43" t="s">
+        <v>81</v>
+      </c>
+      <c r="U43" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" s="1"/>
+      <c r="D44">
+        <v>112</v>
+      </c>
+      <c r="F44">
+        <v>116</v>
+      </c>
+      <c r="H44">
+        <v>115</v>
+      </c>
+      <c r="J44">
+        <v>120</v>
+      </c>
+      <c r="L44">
+        <v>118</v>
+      </c>
+      <c r="N44">
+        <v>112</v>
+      </c>
+      <c r="P44">
+        <v>1</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>1</v>
+      </c>
+      <c r="R44" t="s">
+        <v>62</v>
+      </c>
+      <c r="S44" t="s">
+        <v>77</v>
+      </c>
+      <c r="T44" t="s">
+        <v>81</v>
+      </c>
+      <c r="U44" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P45">
+        <v>1</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>1</v>
+      </c>
+      <c r="R45" t="s">
+        <v>62</v>
+      </c>
+      <c r="S45" t="s">
+        <v>77</v>
+      </c>
+      <c r="T45" t="s">
+        <v>81</v>
+      </c>
+      <c r="U45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>36</v>
+      </c>
+      <c r="F46">
+        <v>38</v>
+      </c>
+      <c r="H46">
+        <v>40</v>
+      </c>
+      <c r="J46">
+        <v>42</v>
+      </c>
+      <c r="L46">
+        <v>44</v>
+      </c>
+      <c r="N46">
+        <v>36</v>
+      </c>
+      <c r="P46">
+        <v>1</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>1</v>
+      </c>
+      <c r="R46" t="s">
+        <v>62</v>
+      </c>
+      <c r="S46" t="s">
+        <v>78</v>
+      </c>
+      <c r="T46" t="s">
+        <v>80</v>
+      </c>
+      <c r="U46" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="2">
+        <v>49500</v>
+      </c>
+      <c r="F47" s="2">
+        <v>49950</v>
+      </c>
+      <c r="H47" s="2">
+        <v>45000</v>
+      </c>
+      <c r="J47" s="2">
+        <v>49940</v>
+      </c>
+      <c r="L47" s="2">
+        <v>45990</v>
+      </c>
+      <c r="N47" s="2">
+        <v>49950</v>
+      </c>
+      <c r="P47">
+        <v>1</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>1</v>
+      </c>
+      <c r="R47" t="s">
+        <v>62</v>
+      </c>
+      <c r="S47" t="s">
+        <v>78</v>
+      </c>
+      <c r="T47" t="s">
+        <v>80</v>
+      </c>
+      <c r="U47" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N48" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P48">
+        <v>1</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>1</v>
+      </c>
+      <c r="R48" t="s">
+        <v>62</v>
+      </c>
+      <c r="S48" t="s">
+        <v>78</v>
+      </c>
+      <c r="T48" t="s">
+        <v>80</v>
+      </c>
+      <c r="U48" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L49" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="N49" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P49">
+        <v>1</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>1</v>
+      </c>
+      <c r="R49" t="s">
+        <v>62</v>
+      </c>
+      <c r="S49" t="s">
+        <v>78</v>
+      </c>
+      <c r="T49" t="s">
+        <v>80</v>
+      </c>
+      <c r="U49" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N50" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P50">
+        <v>1</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>1</v>
+      </c>
+      <c r="R50" t="s">
+        <v>62</v>
+      </c>
+      <c r="S50" t="s">
+        <v>78</v>
+      </c>
+      <c r="T50" t="s">
+        <v>80</v>
+      </c>
+      <c r="U50" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="N51" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P51">
+        <v>1</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>1</v>
+      </c>
+      <c r="R51" t="s">
+        <v>62</v>
+      </c>
+      <c r="S51" t="s">
+        <v>78</v>
+      </c>
+      <c r="T51" t="s">
+        <v>80</v>
+      </c>
+      <c r="U51" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L52" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N52" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P52">
+        <v>1</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>1</v>
+      </c>
+      <c r="R52" t="s">
+        <v>62</v>
+      </c>
+      <c r="S52" t="s">
+        <v>78</v>
+      </c>
+      <c r="T52" t="s">
+        <v>80</v>
+      </c>
+      <c r="U52" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D53">
+        <v>24</v>
+      </c>
+      <c r="F53">
+        <v>22</v>
+      </c>
+      <c r="H53">
+        <v>23</v>
+      </c>
+      <c r="J53">
+        <v>21</v>
+      </c>
+      <c r="L53">
+        <v>20</v>
+      </c>
+      <c r="N53">
+        <v>22</v>
+      </c>
+      <c r="P53">
+        <v>1</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>1</v>
+      </c>
+      <c r="R53" t="s">
+        <v>62</v>
+      </c>
+      <c r="S53" t="s">
+        <v>78</v>
+      </c>
+      <c r="T53" t="s">
+        <v>80</v>
+      </c>
+      <c r="U53" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="N54" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P54">
+        <v>1</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>1</v>
+      </c>
+      <c r="R54" t="s">
+        <v>62</v>
+      </c>
+      <c r="S54" t="s">
+        <v>78</v>
+      </c>
+      <c r="T54" t="s">
+        <v>80</v>
+      </c>
+      <c r="U54" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D55">
+        <v>112</v>
+      </c>
+      <c r="F55">
+        <v>116</v>
+      </c>
+      <c r="H55">
+        <v>115</v>
+      </c>
+      <c r="J55">
+        <v>120</v>
+      </c>
+      <c r="L55">
+        <v>118</v>
+      </c>
+      <c r="N55">
+        <v>112</v>
+      </c>
+      <c r="P55">
+        <v>1</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>1</v>
+      </c>
+      <c r="R55" t="s">
+        <v>62</v>
+      </c>
+      <c r="S55" t="s">
+        <v>78</v>
+      </c>
+      <c r="T55" t="s">
+        <v>80</v>
+      </c>
+      <c r="U55" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L56" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="N56" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P56">
+        <v>1</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>1</v>
+      </c>
+      <c r="R56" t="s">
+        <v>62</v>
+      </c>
+      <c r="S56" t="s">
+        <v>78</v>
+      </c>
+      <c r="T56" t="s">
+        <v>80</v>
+      </c>
+      <c r="U56" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>36</v>
+      </c>
+      <c r="F57">
+        <v>38</v>
+      </c>
+      <c r="H57">
+        <v>40</v>
+      </c>
+      <c r="J57">
+        <v>42</v>
+      </c>
+      <c r="L57">
+        <v>44</v>
+      </c>
+      <c r="N57">
+        <v>36</v>
+      </c>
+      <c r="P57">
+        <v>1</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>1</v>
+      </c>
+      <c r="R57" t="s">
+        <v>62</v>
+      </c>
+      <c r="S57" t="s">
+        <v>79</v>
+      </c>
+      <c r="T57" t="s">
+        <v>61</v>
+      </c>
+      <c r="U57" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D58" s="2">
+        <v>49500</v>
+      </c>
+      <c r="F58" s="2">
+        <v>49950</v>
+      </c>
+      <c r="H58" s="2">
+        <v>45000</v>
+      </c>
+      <c r="J58" s="2">
+        <v>49940</v>
+      </c>
+      <c r="L58" s="2">
+        <v>45990</v>
+      </c>
+      <c r="N58" s="2">
+        <v>49950</v>
+      </c>
+      <c r="P58">
+        <v>1</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>1</v>
+      </c>
+      <c r="R58" t="s">
+        <v>62</v>
+      </c>
+      <c r="S58" t="s">
+        <v>79</v>
+      </c>
+      <c r="T58" t="s">
+        <v>61</v>
+      </c>
+      <c r="U58" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L59" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N59" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P59">
+        <v>1</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>1</v>
+      </c>
+      <c r="R59" t="s">
+        <v>62</v>
+      </c>
+      <c r="S59" t="s">
+        <v>79</v>
+      </c>
+      <c r="T59" t="s">
+        <v>61</v>
+      </c>
+      <c r="U59" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L60" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="N60" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P60">
+        <v>1</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>1</v>
+      </c>
+      <c r="R60" t="s">
+        <v>62</v>
+      </c>
+      <c r="S60" t="s">
+        <v>79</v>
+      </c>
+      <c r="T60" t="s">
+        <v>61</v>
+      </c>
+      <c r="U60" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J61" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L61" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N61" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P61">
+        <v>1</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>1</v>
+      </c>
+      <c r="R61" t="s">
+        <v>62</v>
+      </c>
+      <c r="S61" t="s">
+        <v>79</v>
+      </c>
+      <c r="T61" t="s">
+        <v>61</v>
+      </c>
+      <c r="U61" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L62" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="N62" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P62">
+        <v>1</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>1</v>
+      </c>
+      <c r="R62" t="s">
+        <v>62</v>
+      </c>
+      <c r="S62" t="s">
+        <v>79</v>
+      </c>
+      <c r="T62" t="s">
+        <v>61</v>
+      </c>
+      <c r="U62" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L63" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N63" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P63">
+        <v>1</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>1</v>
+      </c>
+      <c r="R63" t="s">
+        <v>62</v>
+      </c>
+      <c r="S63" t="s">
+        <v>79</v>
+      </c>
+      <c r="T63" t="s">
+        <v>61</v>
+      </c>
+      <c r="U63" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D64">
+        <v>24</v>
+      </c>
+      <c r="F64">
+        <v>22</v>
+      </c>
+      <c r="H64">
+        <v>23</v>
+      </c>
+      <c r="J64">
+        <v>21</v>
+      </c>
+      <c r="L64">
+        <v>20</v>
+      </c>
+      <c r="N64">
+        <v>22</v>
+      </c>
+      <c r="P64">
+        <v>1</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>1</v>
+      </c>
+      <c r="R64" t="s">
+        <v>62</v>
+      </c>
+      <c r="S64" t="s">
+        <v>79</v>
+      </c>
+      <c r="T64" t="s">
+        <v>61</v>
+      </c>
+      <c r="U64" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J65" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L65" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="N65" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P65">
+        <v>1</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>1</v>
+      </c>
+      <c r="R65" t="s">
+        <v>62</v>
+      </c>
+      <c r="S65" t="s">
+        <v>79</v>
+      </c>
+      <c r="T65" t="s">
+        <v>61</v>
+      </c>
+      <c r="U65" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D66">
+        <v>112</v>
+      </c>
+      <c r="F66">
+        <v>116</v>
+      </c>
+      <c r="H66">
+        <v>115</v>
+      </c>
+      <c r="J66">
+        <v>120</v>
+      </c>
+      <c r="L66">
+        <v>118</v>
+      </c>
+      <c r="N66">
+        <v>112</v>
+      </c>
+      <c r="P66">
+        <v>1</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>1</v>
+      </c>
+      <c r="R66" t="s">
+        <v>62</v>
+      </c>
+      <c r="S66" t="s">
+        <v>79</v>
+      </c>
+      <c r="T66" t="s">
+        <v>61</v>
+      </c>
+      <c r="U66" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L67" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="N67" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P67">
+        <v>1</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>1</v>
+      </c>
+      <c r="R67" t="s">
+        <v>62</v>
+      </c>
+      <c r="S67" t="s">
+        <v>79</v>
+      </c>
+      <c r="T67" t="s">
+        <v>61</v>
+      </c>
+      <c r="U67" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>